<commit_message>
feat: add interactive handout view with print support
- Added HandoutView component to display study guides, key terms, equations, and practice quizzes.
- Integrated HandoutView into TopicStudyView with a toggle button.
- Updated setup_data.py to include 'flowchart' content type and sample data (Physics/Work & Energy) with equations and flowcharts.
- Verified render of equations and images within the handout modal.
</commit_message>
<xml_diff>
--- a/public/StudyHub_Complete_Data.xlsx
+++ b/public/StudyHub_Complete_Data.xlsx
@@ -3832,7 +3832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4291,27 +4291,27 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>cont-phys-t3-13</t>
+          <t>cont-phys-t2-13</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>phys-t3-s2</t>
+          <t>phys-t2-s4</t>
         </is>
       </c>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>flowchart</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr">
         <is>
-          <t>Electric Circuits</t>
+          <t>Energy Transformation</t>
         </is>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>A closed loop that allows current to flow. Requires a source (battery), load (bulb), and wires.</t>
+          <t>Visualizing how Potential Energy converts to Kinetic Energy.</t>
         </is>
       </c>
       <c r="F14" s="2" t="n">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1549419163-e380e22784cb?w=800</t>
+          <t>https://mermaid.ink/img/pako:eNpVkMtqwzAQRX9FzKqF_IAeCqWbQsFQAqG7tciyxBZiS0ZSCyX_Xsdf4tJldTPn3DszGtToFCpoeD3pW_QeXwZ0h8-z_sQ12p05sB_tQ4B794dY6_tHj9F59GfW_4E-sB-sO9Z_sBfsC_vAPrAf7IA11v2wF-wL-8A-sB_s4J-x0k5bCg0ZylJyoOQYpZJMy5qrpRCSk0pWUp5S8oOQnJSkC_lLyU_2z7-Xw6GgUCqVbLhQ0pCpkHJYl0qJ4uO6Ff_2B2HqSgM?type=png</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr"/>
@@ -4332,28 +4332,32 @@
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>phys-t3-s3</t>
+          <t>phys-t3-s2</t>
         </is>
       </c>
       <c r="C15" s="2" t="inlineStr">
         <is>
-          <t>formula</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D15" s="2" t="inlineStr">
         <is>
-          <t>Ohm's Law</t>
+          <t>Electric Circuits</t>
         </is>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>V = I \cdot R</t>
+          <t>A closed loop that allows current to flow. Requires a source (battery), load (bulb), and wires.</t>
         </is>
       </c>
       <c r="F15" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G15" s="2" t="inlineStr"/>
+      <c r="G15" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1549419163-e380e22784cb?w=800</t>
+        </is>
+      </c>
       <c r="H15" s="2" t="inlineStr"/>
     </row>
     <row r="16">
@@ -4369,17 +4373,17 @@
       </c>
       <c r="C16" s="2" t="inlineStr">
         <is>
-          <t>real_world</t>
+          <t>formula</t>
         </is>
       </c>
       <c r="D16" s="2" t="inlineStr">
         <is>
-          <t>Resistors</t>
+          <t>Ohm's Law</t>
         </is>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Electronics use resistors to control current so delicate components don't burn out.</t>
+          <t>V = I \cdot R</t>
         </is>
       </c>
       <c r="F16" s="2" t="n">
@@ -4391,27 +4395,27 @@
     <row r="17">
       <c r="A17" s="2" t="inlineStr">
         <is>
-          <t>cont-math-t1-16</t>
+          <t>cont-phys-t3-16</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>math-t1-s2</t>
+          <t>phys-t3-s3</t>
         </is>
       </c>
       <c r="C17" s="2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>real_world</t>
         </is>
       </c>
       <c r="D17" s="2" t="inlineStr">
         <is>
-          <t>What is Algebra?</t>
+          <t>Resistors</t>
         </is>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>Algebra is generalized arithmetic. We use letters to represent numbers we don't know yet.</t>
+          <t>Electronics use resistors to control current so delicate components don't burn out.</t>
         </is>
       </c>
       <c r="F17" s="2" t="n">
@@ -4428,22 +4432,22 @@
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>math-t1-s3</t>
+          <t>math-t1-s2</t>
         </is>
       </c>
       <c r="C18" s="2" t="inlineStr">
         <is>
-          <t>concept_helper</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D18" s="2" t="inlineStr">
         <is>
-          <t>Like Terms</t>
+          <t>What is Algebra?</t>
         </is>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>You can only add terms if they have the same variable part. 2x + 3x = 5x, but 2x + 3y cannot be combined.</t>
+          <t>Algebra is generalized arithmetic. We use letters to represent numbers we don't know yet.</t>
         </is>
       </c>
       <c r="F18" s="2" t="n">
@@ -4465,17 +4469,17 @@
       </c>
       <c r="C19" s="2" t="inlineStr">
         <is>
-          <t>warning</t>
+          <t>concept_helper</t>
         </is>
       </c>
       <c r="D19" s="2" t="inlineStr">
         <is>
-          <t>Watch the powers</t>
+          <t>Like Terms</t>
         </is>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>x and x² are NOT like terms!</t>
+          <t>You can only add terms if they have the same variable part. 2x + 3x = 5x, but 2x + 3y cannot be combined.</t>
         </is>
       </c>
       <c r="F19" s="2" t="n">
@@ -4487,37 +4491,33 @@
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>cont-math-t2-19</t>
+          <t>cont-math-t1-19</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>math-t2-s2</t>
+          <t>math-t1-s3</t>
         </is>
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>warning</t>
         </is>
       </c>
       <c r="D20" s="2" t="inlineStr">
         <is>
-          <t>Triangle Types</t>
+          <t>Watch the powers</t>
         </is>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Triangles can be classified by sides (equilateral, isosceles, scalene) or angles (acute, obtuse, right).</t>
+          <t>x and x² are NOT like terms!</t>
         </is>
       </c>
       <c r="F20" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="2" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1616469829941-c7200ed5dabd?w=800</t>
-        </is>
-      </c>
+      <c r="G20" s="2" t="inlineStr"/>
       <c r="H20" s="2" t="inlineStr"/>
     </row>
     <row r="21">
@@ -4528,28 +4528,32 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>math-t2-s3</t>
+          <t>math-t2-s2</t>
         </is>
       </c>
       <c r="C21" s="2" t="inlineStr">
         <is>
-          <t>formula</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D21" s="2" t="inlineStr">
         <is>
-          <t>Pythagorean Theorem</t>
+          <t>Triangle Types</t>
         </is>
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>a^2 + b^2 = c^2</t>
+          <t>Triangles can be classified by sides (equilateral, isosceles, scalene) or angles (acute, obtuse, right).</t>
         </is>
       </c>
       <c r="F21" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="2" t="inlineStr"/>
+      <c r="G21" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1616469829941-c7200ed5dabd?w=800</t>
+        </is>
+      </c>
       <c r="H21" s="2" t="inlineStr"/>
     </row>
     <row r="22">
@@ -4565,17 +4569,17 @@
       </c>
       <c r="C22" s="2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>formula</t>
         </is>
       </c>
       <c r="D22" s="2" t="inlineStr">
         <is>
-          <t>Usage</t>
+          <t>Pythagorean Theorem</t>
         </is>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Used to find a missing side in a right-angled triangle.</t>
+          <t>a^2 + b^2 = c^2</t>
         </is>
       </c>
       <c r="F22" s="2" t="n">
@@ -4587,12 +4591,12 @@
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>cont-math-t3-22</t>
+          <t>cont-math-t2-22</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>math-t3-s2</t>
+          <t>math-t2-s3</t>
         </is>
       </c>
       <c r="C23" s="2" t="inlineStr">
@@ -4602,12 +4606,12 @@
       </c>
       <c r="D23" s="2" t="inlineStr">
         <is>
-          <t>The Scale</t>
+          <t>Usage</t>
         </is>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
-          <t>Probability ranges from 0 (Impossible) to 1 (Certain).</t>
+          <t>Used to find a missing side in a right-angled triangle.</t>
         </is>
       </c>
       <c r="F23" s="2" t="n">
@@ -4624,22 +4628,22 @@
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>math-t3-s3</t>
+          <t>math-t3-s2</t>
         </is>
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
-          <t>formula</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D24" s="2" t="inlineStr">
         <is>
-          <t>Basic Probability</t>
+          <t>The Scale</t>
         </is>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>P(A) = \frac{\text{favorable outcomes}}{\text{total outcomes}}</t>
+          <t>Probability ranges from 0 (Impossible) to 1 (Certain).</t>
         </is>
       </c>
       <c r="F24" s="2" t="n">
@@ -4661,53 +4665,49 @@
       </c>
       <c r="C25" s="2" t="inlineStr">
         <is>
-          <t>real_world</t>
+          <t>formula</t>
         </is>
       </c>
       <c r="D25" s="2" t="inlineStr">
         <is>
-          <t>Dice</t>
+          <t>Basic Probability</t>
         </is>
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>Rolling a 6 on a standard die has a 1/6 chance.</t>
+          <t>P(A) = \frac{\text{favorable outcomes}}{\text{total outcomes}}</t>
         </is>
       </c>
       <c r="F25" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G25" s="2" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1595113316349-9fa4eb24f884?w=800</t>
-        </is>
-      </c>
+      <c r="G25" s="2" t="inlineStr"/>
       <c r="H25" s="2" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>cont-chem-t1-25</t>
+          <t>cont-math-t3-25</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>chem-t1-s2</t>
+          <t>math-t3-s3</t>
         </is>
       </c>
       <c r="C26" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>real_world</t>
         </is>
       </c>
       <c r="D26" s="2" t="inlineStr">
         <is>
-          <t>Building Blocks</t>
+          <t>Dice</t>
         </is>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>All matter is made of atoms. They are the smallest unit of an element.</t>
+          <t>Rolling a 6 on a standard die has a 1/6 chance.</t>
         </is>
       </c>
       <c r="F26" s="2" t="n">
@@ -4715,7 +4715,7 @@
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1614730341194-75c60740a070?w=800</t>
+          <t>https://images.unsplash.com/photo-1595113316349-9fa4eb24f884?w=800</t>
         </is>
       </c>
       <c r="H26" s="2" t="inlineStr"/>
@@ -4728,28 +4728,32 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>chem-t1-s3</t>
+          <t>chem-t1-s2</t>
         </is>
       </c>
       <c r="C27" s="2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D27" s="2" t="inlineStr">
         <is>
-          <t>Inside the Atom</t>
+          <t>Building Blocks</t>
         </is>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>Protons (+ charge) and Neutrons (no charge) are in the center. Electrons (- charge) zoom around the outside.</t>
+          <t>All matter is made of atoms. They are the smallest unit of an element.</t>
         </is>
       </c>
       <c r="F27" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G27" s="2" t="inlineStr"/>
+      <c r="G27" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1614730341194-75c60740a070?w=800</t>
+        </is>
+      </c>
       <c r="H27" s="2" t="inlineStr"/>
     </row>
     <row r="28">
@@ -4765,64 +4769,60 @@
       </c>
       <c r="C28" s="2" t="inlineStr">
         <is>
-          <t>video</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>Atomic Model</t>
+          <t>Inside the Atom</t>
         </is>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Visualizing the atom.</t>
+          <t>Protons (+ charge) and Neutrons (no charge) are in the center. Electrons (- charge) zoom around the outside.</t>
         </is>
       </c>
       <c r="F28" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="inlineStr"/>
-      <c r="H28" s="2" t="inlineStr">
-        <is>
-          <t>https://www.youtube.com/watch?v=IO9WS_HNmyg</t>
-        </is>
-      </c>
+      <c r="H28" s="2" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>cont-chem-t2-28</t>
+          <t>cont-chem-t1-28</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>chem-t2-s2</t>
+          <t>chem-t1-s3</t>
         </is>
       </c>
       <c r="C29" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>video</t>
         </is>
       </c>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>The Map of Elements</t>
+          <t>Atomic Model</t>
         </is>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>The periodic table organizes all known elements by atomic number and chemical properties.</t>
+          <t>Visualizing the atom.</t>
         </is>
       </c>
       <c r="F29" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G29" s="2" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1603126857599-f6e157fa2fe6?w=800</t>
-        </is>
-      </c>
-      <c r="H29" s="2" t="inlineStr"/>
+      <c r="G29" s="2" t="inlineStr"/>
+      <c r="H29" s="2" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=IO9WS_HNmyg</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="inlineStr">
@@ -4832,28 +4832,32 @@
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>chem-t2-s3</t>
+          <t>chem-t2-s2</t>
         </is>
       </c>
       <c r="C30" s="2" t="inlineStr">
         <is>
-          <t>concept_helper</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>Navigation</t>
+          <t>The Map of Elements</t>
         </is>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Columns are called Groups (elements behave similarly). Rows are called Periods.</t>
+          <t>The periodic table organizes all known elements by atomic number and chemical properties.</t>
         </is>
       </c>
       <c r="F30" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G30" s="2" t="inlineStr"/>
+      <c r="G30" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1603126857599-f6e157fa2fe6?w=800</t>
+        </is>
+      </c>
       <c r="H30" s="2" t="inlineStr"/>
     </row>
     <row r="31">
@@ -4869,17 +4873,17 @@
       </c>
       <c r="C31" s="2" t="inlineStr">
         <is>
-          <t>real_world</t>
+          <t>concept_helper</t>
         </is>
       </c>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>Noble Gases</t>
+          <t>Navigation</t>
         </is>
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>Group 18 elements are "Noble Gases" - they are very stable and don't like to react (like Neon signs).</t>
+          <t>Columns are called Groups (elements behave similarly). Rows are called Periods.</t>
         </is>
       </c>
       <c r="F31" s="2" t="n">
@@ -4891,27 +4895,27 @@
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>cont-chem-t3-31</t>
+          <t>cont-chem-t2-31</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>chem-t3-s2</t>
+          <t>chem-t2-s3</t>
         </is>
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>real_world</t>
         </is>
       </c>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>Stability</t>
+          <t>Noble Gases</t>
         </is>
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>Atoms bond to become stable, usually by getting a full outer shell of electrons.</t>
+          <t>Group 18 elements are "Noble Gases" - they are very stable and don't like to react (like Neon signs).</t>
         </is>
       </c>
       <c r="F32" s="2" t="n">
@@ -4928,7 +4932,7 @@
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>chem-t3-s3</t>
+          <t>chem-t3-s2</t>
         </is>
       </c>
       <c r="C33" s="2" t="inlineStr">
@@ -4938,12 +4942,12 @@
       </c>
       <c r="D33" s="2" t="inlineStr">
         <is>
-          <t>Ionic Bonding</t>
+          <t>Stability</t>
         </is>
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>One atom STEALS electrons from another. Creates + and - ions that attract.</t>
+          <t>Atoms bond to become stable, usually by getting a full outer shell of electrons.</t>
         </is>
       </c>
       <c r="F33" s="2" t="n">
@@ -4970,48 +4974,44 @@
       </c>
       <c r="D34" s="2" t="inlineStr">
         <is>
-          <t>Covalent Bonding</t>
+          <t>Ionic Bonding</t>
         </is>
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Atoms SHARE electrons. Like two people holding hands.</t>
+          <t>One atom STEALS electrons from another. Creates + and - ions that attract.</t>
         </is>
       </c>
       <c r="F34" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G34" s="2" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1532634993-15f421e42ec0?w=800</t>
-        </is>
-      </c>
+      <c r="G34" s="2" t="inlineStr"/>
       <c r="H34" s="2" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="inlineStr">
         <is>
-          <t>cont-bio-t1-34</t>
+          <t>cont-chem-t3-34</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>bio-t1-s2</t>
+          <t>chem-t3-s3</t>
         </is>
       </c>
       <c r="C35" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D35" s="2" t="inlineStr">
         <is>
-          <t>Unit of Life</t>
+          <t>Covalent Bonding</t>
         </is>
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>Cells are the basic structural and functional units of life.</t>
+          <t>Atoms SHARE electrons. Like two people holding hands.</t>
         </is>
       </c>
       <c r="F35" s="2" t="n">
@@ -5019,7 +5019,7 @@
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
-          <t>https://images.unsplash.com/photo-1530210124550-912dc1381cb8?w=800</t>
+          <t>https://images.unsplash.com/photo-1532634993-15f421e42ec0?w=800</t>
         </is>
       </c>
       <c r="H35" s="2" t="inlineStr"/>
@@ -5032,28 +5032,32 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>bio-t1-s3</t>
+          <t>bio-t1-s2</t>
         </is>
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D36" s="2" t="inlineStr">
         <is>
-          <t>Mitochondria</t>
+          <t>Unit of Life</t>
         </is>
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>The POWERHOUSE of the cell. Generates energy (ATP).</t>
+          <t>Cells are the basic structural and functional units of life.</t>
         </is>
       </c>
       <c r="F36" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G36" s="2" t="inlineStr"/>
+      <c r="G36" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1530210124550-912dc1381cb8?w=800</t>
+        </is>
+      </c>
       <c r="H36" s="2" t="inlineStr"/>
     </row>
     <row r="37">
@@ -5074,12 +5078,12 @@
       </c>
       <c r="D37" s="2" t="inlineStr">
         <is>
-          <t>Nucleus</t>
+          <t>Mitochondria</t>
         </is>
       </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>The BRAIN. Contains DNA and controls cell activity.</t>
+          <t>The POWERHOUSE of the cell. Generates energy (ATP).</t>
         </is>
       </c>
       <c r="F37" s="2" t="n">
@@ -5091,37 +5095,33 @@
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>cont-bio-t2-37</t>
+          <t>cont-bio-t1-37</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>bio-t2-s2</t>
+          <t>bio-t1-s3</t>
         </is>
       </c>
       <c r="C38" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>text</t>
         </is>
       </c>
       <c r="D38" s="2" t="inlineStr">
         <is>
-          <t>Blueprint of Life</t>
+          <t>Nucleus</t>
         </is>
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>DNA holds the instructions for building and operating an organism.</t>
+          <t>The BRAIN. Contains DNA and controls cell activity.</t>
         </is>
       </c>
       <c r="F38" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="2" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1576086213369-97a306d36557?w=800</t>
-        </is>
-      </c>
+      <c r="G38" s="2" t="inlineStr"/>
       <c r="H38" s="2" t="inlineStr"/>
     </row>
     <row r="39">
@@ -5132,64 +5132,64 @@
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>bio-t2-s3</t>
+          <t>bio-t2-s2</t>
         </is>
       </c>
       <c r="C39" s="2" t="inlineStr">
         <is>
-          <t>concept_helper</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D39" s="2" t="inlineStr">
         <is>
-          <t>Dominant vs Recessive</t>
+          <t>Blueprint of Life</t>
         </is>
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>Dominant traits (like brown eyes) often hide recessive traits (like blue eyes).</t>
+          <t>DNA holds the instructions for building and operating an organism.</t>
         </is>
       </c>
       <c r="F39" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G39" s="2" t="inlineStr"/>
+      <c r="G39" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1576086213369-97a306d36557?w=800</t>
+        </is>
+      </c>
       <c r="H39" s="2" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>cont-bio-t3-39</t>
+          <t>cont-bio-t2-39</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>bio-t3-s2</t>
+          <t>bio-t2-s3</t>
         </is>
       </c>
       <c r="C40" s="2" t="inlineStr">
         <is>
-          <t>introduction</t>
+          <t>concept_helper</t>
         </is>
       </c>
       <c r="D40" s="2" t="inlineStr">
         <is>
-          <t>Web of Life</t>
+          <t>Dominant vs Recessive</t>
         </is>
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>An ecosystem includes all living things in an area interacting with each other and their environment.</t>
+          <t>Dominant traits (like brown eyes) often hide recessive traits (like blue eyes).</t>
         </is>
       </c>
       <c r="F40" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G40" s="2" t="inlineStr">
-        <is>
-          <t>https://images.unsplash.com/photo-1470071459604-3b5ec3a7fe05?w=800</t>
-        </is>
-      </c>
+      <c r="G40" s="2" t="inlineStr"/>
       <c r="H40" s="2" t="inlineStr"/>
     </row>
     <row r="41">
@@ -5200,29 +5200,65 @@
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>bio-t3-s3</t>
+          <t>bio-t3-s2</t>
         </is>
       </c>
       <c r="C41" s="2" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>introduction</t>
         </is>
       </c>
       <c r="D41" s="2" t="inlineStr">
         <is>
-          <t>Producers vs Consumers</t>
+          <t>Web of Life</t>
         </is>
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>Plants produce energy from sun. Animals consume plants or other animals.</t>
+          <t>An ecosystem includes all living things in an area interacting with each other and their environment.</t>
         </is>
       </c>
       <c r="F41" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G41" s="2" t="inlineStr"/>
+      <c r="G41" s="2" t="inlineStr">
+        <is>
+          <t>https://images.unsplash.com/photo-1470071459604-3b5ec3a7fe05?w=800</t>
+        </is>
+      </c>
       <c r="H41" s="2" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>cont-bio-t3-41</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>bio-t3-s3</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>Producers vs Consumers</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
+        <is>
+          <t>Plants produce energy from sun. Animals consume plants or other animals.</t>
+        </is>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="2" t="inlineStr"/>
+      <c r="H42" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5235,7 +5271,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5246,9 +5282,9 @@
     <col width="16" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="26" customWidth="1" min="3" max="3"/>
-    <col width="21" customWidth="1" min="4" max="4"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
     <col width="19" customWidth="1" min="5" max="5"/>
-    <col width="17" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
     <col width="17" customWidth="1" min="7" max="7"/>
     <col width="19" customWidth="1" min="8" max="8"/>
     <col width="17" customWidth="1" min="9" max="9"/>
@@ -5529,179 +5565,246 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>form-phys-t3-1</t>
+          <t>form-phys-t2-3</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>phys-t3</t>
+          <t>phys-t2</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>V = I \cdot R</t>
+          <t>PE_g = mgh</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Ohm's Law</t>
+          <t>Gravitational Potential Energy</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>PE</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>Voltage</t>
+          <t>Potential Energy</t>
         </is>
       </c>
       <c r="G5" s="2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>J</t>
         </is>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
-          <t>I</t>
+          <t>m</t>
         </is>
       </c>
       <c r="I5" s="2" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>Mass</t>
         </is>
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>kg</t>
         </is>
       </c>
       <c r="K5" s="2" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>h</t>
         </is>
       </c>
       <c r="L5" s="2" t="inlineStr">
         <is>
-          <t>Resistance</t>
+          <t>Height</t>
         </is>
       </c>
       <c r="M5" s="2" t="inlineStr">
         <is>
-          <t>Ω</t>
+          <t>m</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>form-math-t2-1</t>
+          <t>form-phys-t3-1</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>math-t2</t>
+          <t>phys-t3</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>a^2 + b^2 = c^2</t>
+          <t>V = I \cdot R</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Pythagorean Theorem</t>
+          <t>Ohm's Law</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>V</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>Hypotenuse</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="inlineStr"/>
+          <t>Voltage</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>I</t>
         </is>
       </c>
       <c r="I6" s="2" t="inlineStr">
         <is>
-          <t>Side A</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr"/>
+          <t>Current</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="K6" s="2" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>R</t>
         </is>
       </c>
       <c r="L6" s="2" t="inlineStr">
         <is>
-          <t>Side B</t>
-        </is>
-      </c>
-      <c r="M6" s="2" t="inlineStr"/>
+          <t>Resistance</t>
+        </is>
+      </c>
+      <c r="M6" s="2" t="inlineStr">
+        <is>
+          <t>Ω</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>form-math-t3-1</t>
+          <t>form-math-t2-1</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>math-t3</t>
+          <t>math-t2</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>P(A) = \frac{n(A)}{n(S)}</t>
+          <t>a^2 + b^2 = c^2</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Pythagorean Theorem</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>P</t>
+          <t>c</t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Hypotenuse</t>
         </is>
       </c>
       <c r="G7" s="2" t="inlineStr"/>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>n(A)</t>
+          <t>a</t>
         </is>
       </c>
       <c r="I7" s="2" t="inlineStr">
         <is>
-          <t>Favorable</t>
+          <t>Side A</t>
         </is>
       </c>
       <c r="J7" s="2" t="inlineStr"/>
       <c r="K7" s="2" t="inlineStr">
         <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>Side B</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>form-math-t3-1</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>math-t3</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>P(A) = \frac{n(A)}{n(S)}</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr"/>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>n(A)</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>Favorable</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr"/>
+      <c r="K8" s="2" t="inlineStr">
+        <is>
           <t>n(S)</t>
         </is>
       </c>
-      <c r="L7" s="2" t="inlineStr">
+      <c r="L8" s="2" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="M7" s="2" t="inlineStr"/>
+      <c r="M8" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>